<commit_message>
izmenila tabelu sa konekcijama za MOOG
</commit_message>
<xml_diff>
--- a/docs/HIL&DSP_connection.xlsx
+++ b/docs/HIL&DSP_connection.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\struka\DSP\project1\pdfs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\struka\DSP\project1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
+    <sheet name="HIL" sheetId="1" r:id="rId1"/>
+    <sheet name="MOOG" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="45">
   <si>
     <t>DSP IN</t>
   </si>
@@ -147,6 +148,18 @@
   </si>
   <si>
     <t>VAZNO! Povezati AGND HIL-a (analog npr. C1) sa gnd-om launchpad-a</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>5V enc</t>
+  </si>
+  <si>
+    <t>GND enc</t>
+  </si>
+  <si>
+    <t>turn on res</t>
   </si>
 </sst>
 </file>
@@ -324,20 +337,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -388,8 +389,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,336 +704,336 @@
     <col min="9" max="10" width="10.42578125" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" customWidth="1"/>
     <col min="18" max="18" width="10.7109375" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" style="24" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" style="20" customWidth="1"/>
     <col min="20" max="20" width="10.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" style="14" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="24"/>
+      <c r="I2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="5" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="6">
         <v>30</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="8">
         <v>67</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="8">
         <v>5</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="14"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="12">
         <v>28</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="8">
         <v>66</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="8">
         <v>59</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="M5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="14"/>
+      <c r="Q5" s="10"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+      <c r="B6" s="12">
         <v>24</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="12">
         <v>34</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="15">
         <v>0</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="15">
         <v>40</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="14"/>
+      <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="B7" s="12">
         <v>25</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="12">
         <v>51</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="15">
         <v>1</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="15">
         <v>39</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q7" s="14"/>
+      <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="20">
+      <c r="B8" s="16">
         <v>26</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="16">
         <v>53</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="15">
         <v>2</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="15">
         <v>38</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" s="14"/>
+      <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I9" s="19">
+      <c r="I9" s="15">
         <v>3</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="15">
         <v>37</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" s="14"/>
+      <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I10" s="19">
+      <c r="I10" s="15">
         <v>4</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="15">
         <v>36</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="Q10" s="14"/>
+      <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I11" s="19">
+      <c r="I11" s="15">
         <v>5</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="15">
         <v>35</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="M11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="Q11" s="14"/>
+      <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I12" s="12">
+      <c r="I12" s="8">
         <v>6</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="8">
         <v>80</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="18" t="s">
+      <c r="M12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="14"/>
+      <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I13" s="22">
+      <c r="I13" s="18">
         <v>8</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="18">
         <v>78</v>
       </c>
-      <c r="L13" s="22" t="s">
+      <c r="L13" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="23" t="s">
+      <c r="M13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="Q13" s="14"/>
+      <c r="Q13" s="10"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
@@ -1023,553 +1044,553 @@
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
-      <c r="Q14" s="14"/>
+      <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="Q15" s="14"/>
+      <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="Q16" s="14"/>
+      <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
     </row>
     <row r="18" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
     </row>
     <row r="19" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
     </row>
     <row r="20" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
     </row>
     <row r="21" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
     </row>
     <row r="22" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
     </row>
     <row r="23" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
     </row>
     <row r="24" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
     </row>
     <row r="25" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
     </row>
     <row r="26" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
     </row>
     <row r="27" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
     </row>
     <row r="28" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
     </row>
     <row r="29" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
     </row>
     <row r="30" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
     </row>
     <row r="31" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
     </row>
     <row r="32" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
     </row>
     <row r="33" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
     </row>
     <row r="34" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
     </row>
     <row r="35" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-      <c r="T35" s="14"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
     </row>
     <row r="36" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
-      <c r="T36" s="14"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
     </row>
     <row r="37" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
     </row>
     <row r="38" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
     </row>
     <row r="39" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
-      <c r="T39" s="14"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
     </row>
     <row r="40" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
     </row>
     <row r="41" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
-      <c r="T41" s="14"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
     </row>
     <row r="42" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
     </row>
     <row r="43" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
     </row>
     <row r="44" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="10"/>
     </row>
     <row r="45" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
-      <c r="T45" s="14"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10"/>
     </row>
     <row r="46" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
-      <c r="T46" s="14"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="10"/>
+      <c r="T46" s="10"/>
     </row>
     <row r="47" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
-      <c r="T47" s="14"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10"/>
     </row>
     <row r="48" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
-      <c r="T48" s="14"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
+      <c r="S48" s="10"/>
+      <c r="T48" s="10"/>
     </row>
     <row r="49" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="14"/>
+      <c r="Q49" s="10"/>
+      <c r="R49" s="10"/>
+      <c r="S49" s="10"/>
+      <c r="T49" s="10"/>
     </row>
     <row r="50" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q50" s="14"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="14"/>
-      <c r="T50" s="14"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
+      <c r="T50" s="10"/>
     </row>
     <row r="51" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="14"/>
-      <c r="T51" s="14"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+      <c r="S51" s="10"/>
+      <c r="T51" s="10"/>
     </row>
     <row r="52" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="14"/>
-      <c r="T52" s="14"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="10"/>
+      <c r="S52" s="10"/>
+      <c r="T52" s="10"/>
     </row>
     <row r="53" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q53" s="14"/>
-      <c r="R53" s="14"/>
-      <c r="S53" s="14"/>
-      <c r="T53" s="14"/>
+      <c r="Q53" s="10"/>
+      <c r="R53" s="10"/>
+      <c r="S53" s="10"/>
+      <c r="T53" s="10"/>
     </row>
     <row r="54" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="14"/>
-      <c r="T54" s="14"/>
+      <c r="Q54" s="10"/>
+      <c r="R54" s="10"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="10"/>
     </row>
     <row r="55" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q55" s="14"/>
-      <c r="R55" s="14"/>
-      <c r="S55" s="14"/>
-      <c r="T55" s="14"/>
+      <c r="Q55" s="10"/>
+      <c r="R55" s="10"/>
+      <c r="S55" s="10"/>
+      <c r="T55" s="10"/>
     </row>
     <row r="56" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q56" s="14"/>
-      <c r="R56" s="14"/>
-      <c r="S56" s="14"/>
-      <c r="T56" s="14"/>
+      <c r="Q56" s="10"/>
+      <c r="R56" s="10"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="10"/>
     </row>
     <row r="57" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q57" s="14"/>
-      <c r="R57" s="14"/>
-      <c r="S57" s="14"/>
-      <c r="T57" s="14"/>
+      <c r="Q57" s="10"/>
+      <c r="R57" s="10"/>
+      <c r="S57" s="10"/>
+      <c r="T57" s="10"/>
     </row>
     <row r="58" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q58" s="14"/>
-      <c r="R58" s="14"/>
-      <c r="S58" s="14"/>
-      <c r="T58" s="14"/>
+      <c r="Q58" s="10"/>
+      <c r="R58" s="10"/>
+      <c r="S58" s="10"/>
+      <c r="T58" s="10"/>
     </row>
     <row r="59" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q59" s="14"/>
-      <c r="R59" s="14"/>
-      <c r="S59" s="14"/>
-      <c r="T59" s="14"/>
+      <c r="Q59" s="10"/>
+      <c r="R59" s="10"/>
+      <c r="S59" s="10"/>
+      <c r="T59" s="10"/>
     </row>
     <row r="60" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q60" s="14"/>
-      <c r="R60" s="14"/>
-      <c r="S60" s="14"/>
-      <c r="T60" s="14"/>
+      <c r="Q60" s="10"/>
+      <c r="R60" s="10"/>
+      <c r="S60" s="10"/>
+      <c r="T60" s="10"/>
     </row>
     <row r="61" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q61" s="14"/>
-      <c r="R61" s="14"/>
-      <c r="S61" s="14"/>
-      <c r="T61" s="14"/>
+      <c r="Q61" s="10"/>
+      <c r="R61" s="10"/>
+      <c r="S61" s="10"/>
+      <c r="T61" s="10"/>
     </row>
     <row r="62" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q62" s="14"/>
-      <c r="R62" s="14"/>
-      <c r="S62" s="14"/>
-      <c r="T62" s="14"/>
+      <c r="Q62" s="10"/>
+      <c r="R62" s="10"/>
+      <c r="S62" s="10"/>
+      <c r="T62" s="10"/>
     </row>
     <row r="63" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q63" s="14"/>
-      <c r="R63" s="14"/>
-      <c r="S63" s="14"/>
-      <c r="T63" s="14"/>
+      <c r="Q63" s="10"/>
+      <c r="R63" s="10"/>
+      <c r="S63" s="10"/>
+      <c r="T63" s="10"/>
     </row>
     <row r="64" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q64" s="14"/>
-      <c r="R64" s="14"/>
-      <c r="S64" s="14"/>
-      <c r="T64" s="14"/>
+      <c r="Q64" s="10"/>
+      <c r="R64" s="10"/>
+      <c r="S64" s="10"/>
+      <c r="T64" s="10"/>
     </row>
     <row r="65" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q65" s="14"/>
-      <c r="R65" s="14"/>
-      <c r="S65" s="14"/>
-      <c r="T65" s="14"/>
+      <c r="Q65" s="10"/>
+      <c r="R65" s="10"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
     </row>
     <row r="66" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q66" s="14"/>
-      <c r="R66" s="14"/>
-      <c r="S66" s="14"/>
-      <c r="T66" s="14"/>
+      <c r="Q66" s="10"/>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10"/>
     </row>
     <row r="67" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q67" s="14"/>
-      <c r="R67" s="14"/>
-      <c r="S67" s="14"/>
-      <c r="T67" s="14"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+      <c r="S67" s="10"/>
+      <c r="T67" s="10"/>
     </row>
     <row r="68" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q68" s="14"/>
-      <c r="R68" s="14"/>
-      <c r="S68" s="14"/>
-      <c r="T68" s="14"/>
+      <c r="Q68" s="10"/>
+      <c r="R68" s="10"/>
+      <c r="S68" s="10"/>
+      <c r="T68" s="10"/>
     </row>
     <row r="69" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q69" s="14"/>
-      <c r="R69" s="14"/>
-      <c r="S69" s="14"/>
-      <c r="T69" s="14"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="10"/>
+      <c r="T69" s="10"/>
     </row>
     <row r="70" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q70" s="14"/>
-      <c r="R70" s="14"/>
-      <c r="S70" s="14"/>
-      <c r="T70" s="14"/>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="10"/>
+      <c r="S70" s="10"/>
+      <c r="T70" s="10"/>
     </row>
     <row r="71" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q71" s="14"/>
-      <c r="R71" s="14"/>
-      <c r="S71" s="14"/>
-      <c r="T71" s="14"/>
+      <c r="Q71" s="10"/>
+      <c r="R71" s="10"/>
+      <c r="S71" s="10"/>
+      <c r="T71" s="10"/>
     </row>
     <row r="72" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q72" s="14"/>
-      <c r="R72" s="14"/>
-      <c r="S72" s="14"/>
-      <c r="T72" s="14"/>
+      <c r="Q72" s="10"/>
+      <c r="R72" s="10"/>
+      <c r="S72" s="10"/>
+      <c r="T72" s="10"/>
     </row>
     <row r="73" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q73" s="14"/>
-      <c r="R73" s="14"/>
-      <c r="S73" s="14"/>
-      <c r="T73" s="14"/>
+      <c r="Q73" s="10"/>
+      <c r="R73" s="10"/>
+      <c r="S73" s="10"/>
+      <c r="T73" s="10"/>
     </row>
     <row r="74" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q74" s="14"/>
-      <c r="R74" s="14"/>
-      <c r="S74" s="14"/>
-      <c r="T74" s="14"/>
+      <c r="Q74" s="10"/>
+      <c r="R74" s="10"/>
+      <c r="S74" s="10"/>
+      <c r="T74" s="10"/>
     </row>
     <row r="75" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q75" s="14"/>
-      <c r="R75" s="14"/>
-      <c r="S75" s="14"/>
-      <c r="T75" s="14"/>
+      <c r="Q75" s="10"/>
+      <c r="R75" s="10"/>
+      <c r="S75" s="10"/>
+      <c r="T75" s="10"/>
     </row>
     <row r="76" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q76" s="14"/>
-      <c r="R76" s="14"/>
-      <c r="S76" s="14"/>
-      <c r="T76" s="14"/>
+      <c r="Q76" s="10"/>
+      <c r="R76" s="10"/>
+      <c r="S76" s="10"/>
+      <c r="T76" s="10"/>
     </row>
     <row r="77" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q77" s="14"/>
-      <c r="R77" s="14"/>
-      <c r="S77" s="14"/>
-      <c r="T77" s="14"/>
+      <c r="Q77" s="10"/>
+      <c r="R77" s="10"/>
+      <c r="S77" s="10"/>
+      <c r="T77" s="10"/>
     </row>
     <row r="78" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q78" s="14"/>
-      <c r="R78" s="14"/>
-      <c r="S78" s="14"/>
-      <c r="T78" s="14"/>
+      <c r="Q78" s="10"/>
+      <c r="R78" s="10"/>
+      <c r="S78" s="10"/>
+      <c r="T78" s="10"/>
     </row>
     <row r="79" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q79" s="14"/>
-      <c r="R79" s="14"/>
-      <c r="S79" s="14"/>
-      <c r="T79" s="14"/>
+      <c r="Q79" s="10"/>
+      <c r="R79" s="10"/>
+      <c r="S79" s="10"/>
+      <c r="T79" s="10"/>
     </row>
     <row r="80" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q80" s="14"/>
-      <c r="R80" s="14"/>
-      <c r="S80" s="14"/>
-      <c r="T80" s="14"/>
+      <c r="Q80" s="10"/>
+      <c r="R80" s="10"/>
+      <c r="S80" s="10"/>
+      <c r="T80" s="10"/>
     </row>
     <row r="81" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q81" s="14"/>
-      <c r="R81" s="14"/>
-      <c r="S81" s="14"/>
-      <c r="T81" s="14"/>
+      <c r="Q81" s="10"/>
+      <c r="R81" s="10"/>
+      <c r="S81" s="10"/>
+      <c r="T81" s="10"/>
     </row>
     <row r="82" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q82" s="14"/>
-      <c r="R82" s="14"/>
-      <c r="S82" s="14"/>
-      <c r="T82" s="14"/>
+      <c r="Q82" s="10"/>
+      <c r="R82" s="10"/>
+      <c r="S82" s="10"/>
+      <c r="T82" s="10"/>
     </row>
     <row r="83" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q83" s="14"/>
-      <c r="R83" s="14"/>
-      <c r="S83" s="14"/>
-      <c r="T83" s="14"/>
+      <c r="Q83" s="10"/>
+      <c r="R83" s="10"/>
+      <c r="S83" s="10"/>
+      <c r="T83" s="10"/>
     </row>
     <row r="84" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q84" s="14"/>
-      <c r="R84" s="14"/>
-      <c r="S84" s="14"/>
-      <c r="T84" s="14"/>
+      <c r="Q84" s="10"/>
+      <c r="R84" s="10"/>
+      <c r="S84" s="10"/>
+      <c r="T84" s="10"/>
     </row>
     <row r="85" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q85" s="14"/>
-      <c r="R85" s="14"/>
-      <c r="S85" s="14"/>
-      <c r="T85" s="14"/>
+      <c r="Q85" s="10"/>
+      <c r="R85" s="10"/>
+      <c r="S85" s="10"/>
+      <c r="T85" s="10"/>
     </row>
     <row r="86" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q86" s="14"/>
-      <c r="R86" s="14"/>
-      <c r="S86" s="14"/>
-      <c r="T86" s="14"/>
+      <c r="Q86" s="10"/>
+      <c r="R86" s="10"/>
+      <c r="S86" s="10"/>
+      <c r="T86" s="10"/>
     </row>
     <row r="87" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q87" s="14"/>
-      <c r="R87" s="14"/>
-      <c r="S87" s="14"/>
-      <c r="T87" s="14"/>
+      <c r="Q87" s="10"/>
+      <c r="R87" s="10"/>
+      <c r="S87" s="10"/>
+      <c r="T87" s="10"/>
     </row>
     <row r="88" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q88" s="14"/>
-      <c r="R88" s="14"/>
-      <c r="S88" s="14"/>
-      <c r="T88" s="14"/>
+      <c r="Q88" s="10"/>
+      <c r="R88" s="10"/>
+      <c r="S88" s="10"/>
+      <c r="T88" s="10"/>
     </row>
     <row r="89" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q89" s="14"/>
-      <c r="R89" s="14"/>
-      <c r="S89" s="14"/>
-      <c r="T89" s="14"/>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+      <c r="S89" s="10"/>
+      <c r="T89" s="10"/>
     </row>
     <row r="90" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q90" s="14"/>
-      <c r="R90" s="14"/>
-      <c r="S90" s="14"/>
-      <c r="T90" s="14"/>
+      <c r="Q90" s="10"/>
+      <c r="R90" s="10"/>
+      <c r="S90" s="10"/>
+      <c r="T90" s="10"/>
     </row>
     <row r="91" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q91" s="14"/>
-      <c r="R91" s="14"/>
-      <c r="S91" s="14"/>
-      <c r="T91" s="14"/>
+      <c r="Q91" s="10"/>
+      <c r="R91" s="10"/>
+      <c r="S91" s="10"/>
+      <c r="T91" s="10"/>
     </row>
     <row r="92" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q92" s="14"/>
-      <c r="R92" s="14"/>
-      <c r="S92" s="14"/>
-      <c r="T92" s="14"/>
+      <c r="Q92" s="10"/>
+      <c r="R92" s="10"/>
+      <c r="S92" s="10"/>
+      <c r="T92" s="10"/>
     </row>
     <row r="93" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q93" s="14"/>
-      <c r="R93" s="14"/>
-      <c r="S93" s="14"/>
-      <c r="T93" s="14"/>
+      <c r="Q93" s="10"/>
+      <c r="R93" s="10"/>
+      <c r="S93" s="10"/>
+      <c r="T93" s="10"/>
     </row>
     <row r="94" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q94" s="14"/>
-      <c r="R94" s="14"/>
-      <c r="S94" s="14"/>
-      <c r="T94" s="14"/>
+      <c r="Q94" s="10"/>
+      <c r="R94" s="10"/>
+      <c r="S94" s="10"/>
+      <c r="T94" s="10"/>
     </row>
     <row r="95" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q95" s="14"/>
-      <c r="R95" s="14"/>
-      <c r="S95" s="14"/>
-      <c r="T95" s="14"/>
+      <c r="Q95" s="10"/>
+      <c r="R95" s="10"/>
+      <c r="S95" s="10"/>
+      <c r="T95" s="10"/>
     </row>
     <row r="96" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q96" s="14"/>
-      <c r="R96" s="14"/>
-      <c r="S96" s="14"/>
-      <c r="T96" s="14"/>
+      <c r="Q96" s="10"/>
+      <c r="R96" s="10"/>
+      <c r="S96" s="10"/>
+      <c r="T96" s="10"/>
     </row>
     <row r="97" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q97" s="14"/>
-      <c r="R97" s="14"/>
-      <c r="S97" s="14"/>
-      <c r="T97" s="14"/>
+      <c r="Q97" s="10"/>
+      <c r="R97" s="10"/>
+      <c r="S97" s="10"/>
+      <c r="T97" s="10"/>
     </row>
     <row r="98" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q98" s="14"/>
-      <c r="R98" s="14"/>
-      <c r="S98" s="14"/>
-      <c r="T98" s="14"/>
+      <c r="Q98" s="10"/>
+      <c r="R98" s="10"/>
+      <c r="S98" s="10"/>
+      <c r="T98" s="10"/>
     </row>
     <row r="99" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q99" s="14"/>
-      <c r="R99" s="14"/>
-      <c r="S99" s="14"/>
-      <c r="T99" s="14"/>
+      <c r="Q99" s="10"/>
+      <c r="R99" s="10"/>
+      <c r="S99" s="10"/>
+      <c r="T99" s="10"/>
     </row>
     <row r="100" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q100" s="14"/>
-      <c r="R100" s="14"/>
-      <c r="S100" s="14"/>
-      <c r="T100" s="14"/>
+      <c r="Q100" s="10"/>
+      <c r="R100" s="10"/>
+      <c r="S100" s="10"/>
+      <c r="T100" s="10"/>
     </row>
     <row r="101" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q101" s="14"/>
-      <c r="R101" s="14"/>
-      <c r="S101" s="14"/>
-      <c r="T101" s="14"/>
+      <c r="Q101" s="10"/>
+      <c r="R101" s="10"/>
+      <c r="S101" s="10"/>
+      <c r="T101" s="10"/>
     </row>
     <row r="102" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q102" s="14"/>
-      <c r="R102" s="14"/>
-      <c r="S102" s="14"/>
-      <c r="T102" s="14"/>
+      <c r="Q102" s="10"/>
+      <c r="R102" s="10"/>
+      <c r="S102" s="10"/>
+      <c r="T102" s="10"/>
     </row>
     <row r="103" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q103" s="14"/>
-      <c r="R103" s="14"/>
-      <c r="S103" s="14"/>
-      <c r="T103" s="14"/>
+      <c r="Q103" s="10"/>
+      <c r="R103" s="10"/>
+      <c r="S103" s="10"/>
+      <c r="T103" s="10"/>
     </row>
     <row r="104" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q104" s="14"/>
-      <c r="R104" s="14"/>
-      <c r="S104" s="14"/>
-      <c r="T104" s="14"/>
+      <c r="Q104" s="10"/>
+      <c r="R104" s="10"/>
+      <c r="S104" s="10"/>
+      <c r="T104" s="10"/>
     </row>
     <row r="105" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q105" s="14"/>
-      <c r="R105" s="14"/>
-      <c r="S105" s="14"/>
-      <c r="T105" s="14"/>
+      <c r="Q105" s="10"/>
+      <c r="R105" s="10"/>
+      <c r="S105" s="10"/>
+      <c r="T105" s="10"/>
     </row>
     <row r="106" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q106" s="14"/>
-      <c r="R106" s="14"/>
-      <c r="S106" s="14"/>
-      <c r="T106" s="14"/>
+      <c r="Q106" s="10"/>
+      <c r="R106" s="10"/>
+      <c r="S106" s="10"/>
+      <c r="T106" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1581,4 +1602,872 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="7" max="8" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" style="20" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="G2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6">
+        <v>30</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="29">
+        <v>67</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="29">
+        <v>5</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="10"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="12">
+        <v>28</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8">
+        <v>66</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="8">
+        <v>59</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="10"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>54</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="15">
+        <v>40</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="10"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
+        <v>55</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="12">
+        <v>2</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="15">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="15">
+        <v>39</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="10"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
+        <v>57</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="12">
+        <v>3</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="15">
+        <v>2</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="15">
+        <v>38</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" s="10"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="26">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="15">
+        <v>3</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="15">
+        <v>37</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="10"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="27">
+        <v>5</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="15">
+        <v>4</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="15">
+        <v>36</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="10"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G11" s="15">
+        <v>5</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="15">
+        <v>35</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="10"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G12" s="8">
+        <v>6</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="8">
+        <v>80</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="10"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G13" s="8">
+        <v>8</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="8">
+        <v>78</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" s="10"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="G14" s="28">
+        <v>16</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="28">
+        <v>33</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="N14" s="10"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="10"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="10"/>
+    </row>
+    <row r="17" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+    </row>
+    <row r="18" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+    </row>
+    <row r="19" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+    </row>
+    <row r="20" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+    </row>
+    <row r="21" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+    </row>
+    <row r="22" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+    </row>
+    <row r="23" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+    </row>
+    <row r="24" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+    </row>
+    <row r="26" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+    </row>
+    <row r="27" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+    </row>
+    <row r="28" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+    </row>
+    <row r="29" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+    </row>
+    <row r="30" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+    </row>
+    <row r="31" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+    </row>
+    <row r="32" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+    </row>
+    <row r="33" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+    </row>
+    <row r="34" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+    </row>
+    <row r="35" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+    </row>
+    <row r="36" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+    </row>
+    <row r="37" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+    </row>
+    <row r="38" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+    </row>
+    <row r="39" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+    </row>
+    <row r="40" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+    </row>
+    <row r="41" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+    </row>
+    <row r="42" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+    </row>
+    <row r="43" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+    </row>
+    <row r="44" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+    </row>
+    <row r="45" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+    </row>
+    <row r="46" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+    </row>
+    <row r="47" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+    </row>
+    <row r="48" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+    </row>
+    <row r="49" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
+    </row>
+    <row r="50" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+    </row>
+    <row r="51" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+    </row>
+    <row r="52" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N52" s="10"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+    </row>
+    <row r="53" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+    </row>
+    <row r="54" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10"/>
+    </row>
+    <row r="55" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N55" s="10"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="10"/>
+    </row>
+    <row r="56" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N56" s="10"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="10"/>
+    </row>
+    <row r="57" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N57" s="10"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="10"/>
+      <c r="Q57" s="10"/>
+    </row>
+    <row r="58" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N58" s="10"/>
+      <c r="O58" s="10"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
+    </row>
+    <row r="59" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N59" s="10"/>
+      <c r="O59" s="10"/>
+      <c r="P59" s="10"/>
+      <c r="Q59" s="10"/>
+    </row>
+    <row r="60" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N60" s="10"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="10"/>
+    </row>
+    <row r="61" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N61" s="10"/>
+      <c r="O61" s="10"/>
+      <c r="P61" s="10"/>
+      <c r="Q61" s="10"/>
+    </row>
+    <row r="62" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N62" s="10"/>
+      <c r="O62" s="10"/>
+      <c r="P62" s="10"/>
+      <c r="Q62" s="10"/>
+    </row>
+    <row r="63" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N63" s="10"/>
+      <c r="O63" s="10"/>
+      <c r="P63" s="10"/>
+      <c r="Q63" s="10"/>
+    </row>
+    <row r="64" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N64" s="10"/>
+      <c r="O64" s="10"/>
+      <c r="P64" s="10"/>
+      <c r="Q64" s="10"/>
+    </row>
+    <row r="65" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N65" s="10"/>
+      <c r="O65" s="10"/>
+      <c r="P65" s="10"/>
+      <c r="Q65" s="10"/>
+    </row>
+    <row r="66" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N66" s="10"/>
+      <c r="O66" s="10"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="10"/>
+    </row>
+    <row r="67" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N67" s="10"/>
+      <c r="O67" s="10"/>
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+    </row>
+    <row r="68" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N68" s="10"/>
+      <c r="O68" s="10"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="10"/>
+    </row>
+    <row r="69" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+    </row>
+    <row r="70" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N70" s="10"/>
+      <c r="O70" s="10"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="10"/>
+    </row>
+    <row r="71" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N71" s="10"/>
+      <c r="O71" s="10"/>
+      <c r="P71" s="10"/>
+      <c r="Q71" s="10"/>
+    </row>
+    <row r="72" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N72" s="10"/>
+      <c r="O72" s="10"/>
+      <c r="P72" s="10"/>
+      <c r="Q72" s="10"/>
+    </row>
+    <row r="73" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N73" s="10"/>
+      <c r="O73" s="10"/>
+      <c r="P73" s="10"/>
+      <c r="Q73" s="10"/>
+    </row>
+    <row r="74" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N74" s="10"/>
+      <c r="O74" s="10"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="10"/>
+    </row>
+    <row r="75" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N75" s="10"/>
+      <c r="O75" s="10"/>
+      <c r="P75" s="10"/>
+      <c r="Q75" s="10"/>
+    </row>
+    <row r="76" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N76" s="10"/>
+      <c r="O76" s="10"/>
+      <c r="P76" s="10"/>
+      <c r="Q76" s="10"/>
+    </row>
+    <row r="77" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N77" s="10"/>
+      <c r="O77" s="10"/>
+      <c r="P77" s="10"/>
+      <c r="Q77" s="10"/>
+    </row>
+    <row r="78" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N78" s="10"/>
+      <c r="O78" s="10"/>
+      <c r="P78" s="10"/>
+      <c r="Q78" s="10"/>
+    </row>
+    <row r="79" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N79" s="10"/>
+      <c r="O79" s="10"/>
+      <c r="P79" s="10"/>
+      <c r="Q79" s="10"/>
+    </row>
+    <row r="80" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N80" s="10"/>
+      <c r="O80" s="10"/>
+      <c r="P80" s="10"/>
+      <c r="Q80" s="10"/>
+    </row>
+    <row r="81" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N81" s="10"/>
+      <c r="O81" s="10"/>
+      <c r="P81" s="10"/>
+      <c r="Q81" s="10"/>
+    </row>
+    <row r="82" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N82" s="10"/>
+      <c r="O82" s="10"/>
+      <c r="P82" s="10"/>
+      <c r="Q82" s="10"/>
+    </row>
+    <row r="83" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N83" s="10"/>
+      <c r="O83" s="10"/>
+      <c r="P83" s="10"/>
+      <c r="Q83" s="10"/>
+    </row>
+    <row r="84" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N84" s="10"/>
+      <c r="O84" s="10"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="10"/>
+    </row>
+    <row r="85" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N85" s="10"/>
+      <c r="O85" s="10"/>
+      <c r="P85" s="10"/>
+      <c r="Q85" s="10"/>
+    </row>
+    <row r="86" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N86" s="10"/>
+      <c r="O86" s="10"/>
+      <c r="P86" s="10"/>
+      <c r="Q86" s="10"/>
+    </row>
+    <row r="87" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N87" s="10"/>
+      <c r="O87" s="10"/>
+      <c r="P87" s="10"/>
+      <c r="Q87" s="10"/>
+    </row>
+    <row r="88" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N88" s="10"/>
+      <c r="O88" s="10"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="10"/>
+    </row>
+    <row r="89" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N89" s="10"/>
+      <c r="O89" s="10"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="10"/>
+    </row>
+    <row r="90" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N90" s="10"/>
+      <c r="O90" s="10"/>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="10"/>
+    </row>
+    <row r="91" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N91" s="10"/>
+      <c r="O91" s="10"/>
+      <c r="P91" s="10"/>
+      <c r="Q91" s="10"/>
+    </row>
+    <row r="92" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N92" s="10"/>
+      <c r="O92" s="10"/>
+      <c r="P92" s="10"/>
+      <c r="Q92" s="10"/>
+    </row>
+    <row r="93" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N93" s="10"/>
+      <c r="O93" s="10"/>
+      <c r="P93" s="10"/>
+      <c r="Q93" s="10"/>
+    </row>
+    <row r="94" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N94" s="10"/>
+      <c r="O94" s="10"/>
+      <c r="P94" s="10"/>
+      <c r="Q94" s="10"/>
+    </row>
+    <row r="95" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N95" s="10"/>
+      <c r="O95" s="10"/>
+      <c r="P95" s="10"/>
+      <c r="Q95" s="10"/>
+    </row>
+    <row r="96" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N96" s="10"/>
+      <c r="O96" s="10"/>
+      <c r="P96" s="10"/>
+      <c r="Q96" s="10"/>
+    </row>
+    <row r="97" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N97" s="10"/>
+      <c r="O97" s="10"/>
+      <c r="P97" s="10"/>
+      <c r="Q97" s="10"/>
+    </row>
+    <row r="98" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N98" s="10"/>
+      <c r="O98" s="10"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="10"/>
+    </row>
+    <row r="99" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N99" s="10"/>
+      <c r="O99" s="10"/>
+      <c r="P99" s="10"/>
+      <c r="Q99" s="10"/>
+    </row>
+    <row r="100" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N100" s="10"/>
+      <c r="O100" s="10"/>
+      <c r="P100" s="10"/>
+      <c r="Q100" s="10"/>
+    </row>
+    <row r="101" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N101" s="10"/>
+      <c r="O101" s="10"/>
+      <c r="P101" s="10"/>
+      <c r="Q101" s="10"/>
+    </row>
+    <row r="102" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N102" s="10"/>
+      <c r="O102" s="10"/>
+      <c r="P102" s="10"/>
+      <c r="Q102" s="10"/>
+    </row>
+    <row r="103" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N103" s="10"/>
+      <c r="O103" s="10"/>
+      <c r="P103" s="10"/>
+      <c r="Q103" s="10"/>
+    </row>
+    <row r="104" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N104" s="10"/>
+      <c r="O104" s="10"/>
+      <c r="P104" s="10"/>
+      <c r="Q104" s="10"/>
+    </row>
+    <row r="105" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N105" s="10"/>
+      <c r="O105" s="10"/>
+      <c r="P105" s="10"/>
+      <c r="Q105" s="10"/>
+    </row>
+    <row r="106" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N106" s="10"/>
+      <c r="O106" s="10"/>
+      <c r="P106" s="10"/>
+      <c r="Q106" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>